<commit_message>
title page & headers
</commit_message>
<xml_diff>
--- a/SRS/requirements.xlsx
+++ b/SRS/requirements.xlsx
@@ -1134,10 +1134,6 @@
     <t>На странице корзины выводятся товары, отобранные для заказа, ввод номера ваучера, общая сумма заказа с учетом скидок (для акций), рекомендуемые товары, перечень потенциальных акций на корзину целиком</t>
   </si>
   <si>
-    <t>Все точки самовывоза - есть склады. Существуют склады, не являющиеся
-точками самовывоза</t>
-  </si>
-  <si>
     <t>Нажатие на "Купить" для набора приводит к помещению в корзину сразу нескольких артикулов. Далее из корзины можно удалить любой товар из набора</t>
   </si>
   <si>
@@ -1145,6 +1141,9 @@
   </si>
   <si>
     <t>Интеграция с внутренними ИС ТехноНИКОЛЬ</t>
+  </si>
+  <si>
+    <t>Все точки самовывоза - есть склады. Существуют склады, не являющиеся точками самовывоза</t>
   </si>
 </sst>
 </file>
@@ -1530,8 +1529,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:S766"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="D167" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N176" sqref="N176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,7 +1708,7 @@
         <v>12</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>2</v>
@@ -3136,7 +3135,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>31</v>
@@ -3196,7 +3195,7 @@
         <v>18</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>31</v>
@@ -3256,7 +3255,7 @@
         <v>18</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>31</v>
@@ -3316,7 +3315,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>31</v>
@@ -3376,7 +3375,7 @@
         <v>18</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>31</v>
@@ -3436,7 +3435,7 @@
         <v>18</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>31</v>
@@ -3496,7 +3495,7 @@
         <v>18</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>31</v>
@@ -3556,7 +3555,7 @@
         <v>18</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>31</v>
@@ -3616,7 +3615,7 @@
         <v>18</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>31</v>
@@ -3676,7 +3675,7 @@
         <v>18</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>31</v>
@@ -7805,7 +7804,7 @@
         <v>12</v>
       </c>
       <c r="N107" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O107" s="1" t="s">
         <v>2</v>
@@ -8665,7 +8664,7 @@
         <v>17</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>18</v>
@@ -8722,7 +8721,7 @@
         <v>17</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>18</v>
@@ -8779,7 +8778,7 @@
         <v>17</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>18</v>
@@ -8836,7 +8835,7 @@
         <v>17</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>18</v>
@@ -8893,7 +8892,7 @@
         <v>17</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>18</v>
@@ -8950,7 +8949,7 @@
         <v>17</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>18</v>
@@ -9007,7 +9006,7 @@
         <v>17</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>18</v>
@@ -9067,7 +9066,7 @@
         <v>17</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>18</v>
@@ -9127,7 +9126,7 @@
         <v>17</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>18</v>
@@ -9187,7 +9186,7 @@
         <v>17</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>18</v>
@@ -9247,7 +9246,7 @@
         <v>17</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>18</v>
@@ -9307,7 +9306,7 @@
         <v>17</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>18</v>
@@ -9367,7 +9366,7 @@
         <v>17</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>18</v>
@@ -9427,7 +9426,7 @@
         <v>17</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>18</v>
@@ -9487,7 +9486,7 @@
         <v>17</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>18</v>
@@ -9547,7 +9546,7 @@
         <v>17</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>18</v>
@@ -9607,7 +9606,7 @@
         <v>17</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>18</v>
@@ -9667,7 +9666,7 @@
         <v>17</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>18</v>
@@ -9727,7 +9726,7 @@
         <v>17</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>18</v>
@@ -11864,7 +11863,7 @@
         <v>12</v>
       </c>
       <c r="N176" s="4" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="O176" s="1" t="s">
         <v>2</v>

</xml_diff>